<commit_message>
testing scripts complete, continued work on runavalanceactivity
</commit_message>
<xml_diff>
--- a/varsomdata/input/aval_dl_configuration.xlsx
+++ b/varsomdata/input/aval_dl_configuration.xlsx
@@ -7,9 +7,9 @@
     <workbookView xWindow="-25245" yWindow="180" windowWidth="25605" windowHeight="16065" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Ark1" sheetId="1" r:id="rId1"/>
+    <sheet name="aval_dl_configuration" sheetId="1" r:id="rId1"/>
     <sheet name="Mapping" sheetId="2" r:id="rId2"/>
-    <sheet name="Ark2" sheetId="3" r:id="rId3"/>
+    <sheet name="aval_dl_order_of_size_and_num" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
   <si>
     <t>x</t>
   </si>
@@ -184,6 +184,9 @@
   <si>
     <t>betyr mer alvorlig situasjon.</t>
   </si>
+  <si>
+    <t>order</t>
+  </si>
 </sst>
 </file>
 
@@ -718,7 +721,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -784,14 +787,8 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment textRotation="180"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -799,6 +796,24 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="389">
     <cellStyle name="Benyttet hyperkobling" xfId="3" builtinId="9" hidden="1"/>
@@ -7614,7 +7629,7 @@
   <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" customHeight="1"/>
@@ -7705,7 +7720,7 @@
       <c r="E5" s="4">
         <v>300</v>
       </c>
-      <c r="M5" s="30" t="str">
+      <c r="M5" s="28" t="str">
         <f>D8</f>
         <v>5 - Svaert store</v>
       </c>
@@ -7736,7 +7751,7 @@
         <v>400</v>
       </c>
       <c r="K6" s="4"/>
-      <c r="M6" s="30" t="str">
+      <c r="M6" s="28" t="str">
         <f>D7</f>
         <v>4 - Store</v>
       </c>
@@ -7767,7 +7782,7 @@
         <v>500</v>
       </c>
       <c r="K7" s="4"/>
-      <c r="M7" s="30" t="str">
+      <c r="M7" s="28" t="str">
         <f>D6</f>
         <v>3 - Middels</v>
       </c>
@@ -7798,7 +7813,7 @@
         <v>600</v>
       </c>
       <c r="K8" s="4"/>
-      <c r="M8" s="30" t="str">
+      <c r="M8" s="28" t="str">
         <f>D5</f>
         <v>2 - Smaa</v>
       </c>
@@ -7827,7 +7842,7 @@
       </c>
       <c r="F9" s="6"/>
       <c r="K9" s="4"/>
-      <c r="M9" s="30" t="str">
+      <c r="M9" s="28" t="str">
         <f>D4</f>
         <v>1 - Harmloest</v>
       </c>
@@ -7864,16 +7879,16 @@
       <c r="M10" s="5">
         <v>2</v>
       </c>
-      <c r="N10" s="31">
+      <c r="N10" s="29">
         <v>2</v>
       </c>
-      <c r="O10" s="31">
+      <c r="O10" s="29">
         <v>3</v>
       </c>
-      <c r="P10" s="31">
+      <c r="P10" s="29">
         <v>4</v>
       </c>
-      <c r="Q10" s="31">
+      <c r="Q10" s="29">
         <v>5</v>
       </c>
     </row>
@@ -7890,30 +7905,30 @@
       <c r="E11" s="4">
         <v>200</v>
       </c>
-      <c r="L11" s="29" t="str">
+      <c r="L11" s="30" t="str">
         <f>D10</f>
         <v>Ingen</v>
       </c>
-      <c r="M11" s="27" t="s">
+      <c r="M11" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="N11" s="29" t="str">
+      <c r="N11" s="30" t="str">
         <f>D12</f>
         <v>Ett (1)</v>
       </c>
-      <c r="O11" s="29" t="str">
+      <c r="O11" s="30" t="str">
         <f>D13</f>
         <v>Noen (2-5)</v>
       </c>
-      <c r="P11" s="29" t="str">
+      <c r="P11" s="30" t="str">
         <f>D14</f>
         <v>Flere (6-10)</v>
       </c>
-      <c r="Q11" s="29" t="str">
+      <c r="Q11" s="30" t="str">
         <f>D15</f>
         <v>Mange (10 eller mer)</v>
       </c>
-      <c r="S11" s="28"/>
+      <c r="S11" s="27"/>
     </row>
     <row r="12" spans="1:19" ht="15" customHeight="1">
       <c r="B12" s="4" t="s">
@@ -7928,12 +7943,12 @@
       <c r="E12" s="4">
         <v>300</v>
       </c>
-      <c r="L12" s="29"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="30"/>
       <c r="S12" s="26"/>
     </row>
     <row r="13" spans="1:19" ht="15" customHeight="1">
@@ -7949,12 +7964,12 @@
       <c r="E13" s="4">
         <v>400</v>
       </c>
-      <c r="L13" s="29"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="29"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="30"/>
     </row>
     <row r="14" spans="1:19" ht="15" customHeight="1">
       <c r="B14" s="4" t="s">
@@ -7969,12 +7984,12 @@
       <c r="E14" s="4">
         <v>500</v>
       </c>
-      <c r="L14" s="29"/>
-      <c r="M14" s="27"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="29"/>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="29"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="30"/>
     </row>
     <row r="15" spans="1:19" ht="15" customHeight="1">
       <c r="B15" s="4" t="s">
@@ -7989,12 +8004,12 @@
       <c r="E15" s="3">
         <v>600</v>
       </c>
-      <c r="L15" s="29"/>
-      <c r="M15" s="27"/>
-      <c r="N15" s="29"/>
-      <c r="O15" s="29"/>
-      <c r="P15" s="29"/>
-      <c r="Q15" s="29"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="30"/>
     </row>
     <row r="16" spans="1:19" ht="15" customHeight="1">
       <c r="A16" s="6" t="s">
@@ -8007,12 +8022,12 @@
         <v>0</v>
       </c>
       <c r="F16" s="6"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="29"/>
-      <c r="O16" s="29"/>
-      <c r="P16" s="29"/>
-      <c r="Q16" s="29"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="30"/>
     </row>
     <row r="17" spans="1:17" ht="15" customHeight="1">
       <c r="B17" s="4" t="s">
@@ -8027,12 +8042,12 @@
       <c r="E17" s="4">
         <v>0</v>
       </c>
-      <c r="L17" s="29"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="29"/>
-      <c r="O17" s="29"/>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="29"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="30"/>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="30"/>
     </row>
     <row r="18" spans="1:17" ht="15" customHeight="1">
       <c r="B18" s="4" t="s">
@@ -8047,12 +8062,12 @@
       <c r="E18" s="4">
         <v>600</v>
       </c>
-      <c r="L18" s="29"/>
-      <c r="M18" s="27"/>
-      <c r="N18" s="29"/>
-      <c r="O18" s="29"/>
-      <c r="P18" s="29"/>
-      <c r="Q18" s="29"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="30"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="30"/>
     </row>
     <row r="19" spans="1:17" ht="15" customHeight="1">
       <c r="B19" s="4" t="s">
@@ -8067,12 +8082,12 @@
       <c r="E19" s="4">
         <v>1200</v>
       </c>
-      <c r="L19" s="29"/>
-      <c r="M19" s="27"/>
-      <c r="N19" s="29"/>
-      <c r="O19" s="29"/>
-      <c r="P19" s="29"/>
-      <c r="Q19" s="29"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="30"/>
+      <c r="P19" s="30"/>
+      <c r="Q19" s="30"/>
     </row>
     <row r="20" spans="1:17" ht="15" customHeight="1">
       <c r="B20" s="4" t="s">
@@ -8204,14 +8219,343 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J18"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20" style="16" customWidth="1"/>
+    <col min="2" max="2" width="16.625" style="35" customWidth="1"/>
+    <col min="3" max="3" width="11" style="5"/>
+    <col min="4" max="16384" width="11" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="32" t="str">
+        <f>Mapping!A9</f>
+        <v>EstimatedNum</v>
+      </c>
+      <c r="B1" s="33" t="str">
+        <f>Mapping!A2</f>
+        <v>DestructiveSize</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="16" t="str">
+        <f>Mapping!L11</f>
+        <v>Ingen</v>
+      </c>
+      <c r="B2" s="35" t="str">
+        <f>A2</f>
+        <v>Ingen</v>
+      </c>
+      <c r="C2" s="5">
+        <f>Mapping!L10</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="36" t="str">
+        <f>Mapping!M11</f>
+        <v>Observert faretegn</v>
+      </c>
+      <c r="B3" s="37" t="str">
+        <f>A3</f>
+        <v>Observert faretegn</v>
+      </c>
+      <c r="C3" s="5">
+        <f>Mapping!M10</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="16" t="str">
+        <f>Mapping!N$11</f>
+        <v>Ett (1)</v>
+      </c>
+      <c r="B4" s="37" t="str">
+        <f>Mapping!M$9</f>
+        <v>1 - Harmloest</v>
+      </c>
+      <c r="C4" s="5">
+        <f>Mapping!$N9</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="16" t="str">
+        <f>Mapping!O$11</f>
+        <v>Noen (2-5)</v>
+      </c>
+      <c r="B5" s="37" t="str">
+        <f>Mapping!M$9</f>
+        <v>1 - Harmloest</v>
+      </c>
+      <c r="C5" s="5">
+        <f>Mapping!$O9</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="16" t="str">
+        <f>Mapping!P$11</f>
+        <v>Flere (6-10)</v>
+      </c>
+      <c r="B6" s="37" t="str">
+        <f>Mapping!M$9</f>
+        <v>1 - Harmloest</v>
+      </c>
+      <c r="C6" s="5">
+        <f>Mapping!$P9</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="16" t="str">
+        <f>Mapping!Q$11</f>
+        <v>Mange (10 eller mer)</v>
+      </c>
+      <c r="B7" s="37" t="str">
+        <f>Mapping!M$9</f>
+        <v>1 - Harmloest</v>
+      </c>
+      <c r="C7" s="5">
+        <f>Mapping!$Q9</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="16" t="str">
+        <f>Mapping!N$11</f>
+        <v>Ett (1)</v>
+      </c>
+      <c r="B8" s="37" t="str">
+        <f>Mapping!M$8</f>
+        <v>2 - Smaa</v>
+      </c>
+      <c r="C8" s="5">
+        <f>Mapping!$N8</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="16" t="str">
+        <f>Mapping!O$11</f>
+        <v>Noen (2-5)</v>
+      </c>
+      <c r="B9" s="37" t="str">
+        <f>Mapping!M$8</f>
+        <v>2 - Smaa</v>
+      </c>
+      <c r="C9" s="5">
+        <f>Mapping!$O8</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="16" t="str">
+        <f>Mapping!P$11</f>
+        <v>Flere (6-10)</v>
+      </c>
+      <c r="B10" s="37" t="str">
+        <f>Mapping!M$8</f>
+        <v>2 - Smaa</v>
+      </c>
+      <c r="C10" s="5">
+        <f>Mapping!$P8</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="16" t="str">
+        <f>Mapping!Q$11</f>
+        <v>Mange (10 eller mer)</v>
+      </c>
+      <c r="B11" s="37" t="str">
+        <f>Mapping!M$8</f>
+        <v>2 - Smaa</v>
+      </c>
+      <c r="C11" s="5">
+        <f>Mapping!$Q8</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="16" t="str">
+        <f>Mapping!N$11</f>
+        <v>Ett (1)</v>
+      </c>
+      <c r="B12" s="37" t="str">
+        <f>Mapping!M$7</f>
+        <v>3 - Middels</v>
+      </c>
+      <c r="C12" s="5">
+        <f>Mapping!$N7</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="16" t="str">
+        <f>Mapping!O$11</f>
+        <v>Noen (2-5)</v>
+      </c>
+      <c r="B13" s="37" t="str">
+        <f>Mapping!M$7</f>
+        <v>3 - Middels</v>
+      </c>
+      <c r="C13" s="5">
+        <f>Mapping!$O7</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="16" t="str">
+        <f>Mapping!P$11</f>
+        <v>Flere (6-10)</v>
+      </c>
+      <c r="B14" s="37" t="str">
+        <f>Mapping!M$7</f>
+        <v>3 - Middels</v>
+      </c>
+      <c r="C14" s="5">
+        <f>Mapping!$P7</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="16" t="str">
+        <f>Mapping!Q$11</f>
+        <v>Mange (10 eller mer)</v>
+      </c>
+      <c r="B15" s="37" t="str">
+        <f>Mapping!M$7</f>
+        <v>3 - Middels</v>
+      </c>
+      <c r="C15" s="5">
+        <f>Mapping!$Q7</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="16" t="str">
+        <f>Mapping!N$11</f>
+        <v>Ett (1)</v>
+      </c>
+      <c r="B16" s="37" t="str">
+        <f>Mapping!M$6</f>
+        <v>4 - Store</v>
+      </c>
+      <c r="C16" s="5">
+        <f>Mapping!$N6</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="16" t="str">
+        <f>Mapping!O$11</f>
+        <v>Noen (2-5)</v>
+      </c>
+      <c r="B17" s="37" t="str">
+        <f>Mapping!M$6</f>
+        <v>4 - Store</v>
+      </c>
+      <c r="C17" s="5">
+        <f>Mapping!$O6</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="16" t="str">
+        <f>Mapping!P$11</f>
+        <v>Flere (6-10)</v>
+      </c>
+      <c r="B18" s="37" t="str">
+        <f>Mapping!M$6</f>
+        <v>4 - Store</v>
+      </c>
+      <c r="C18" s="5">
+        <f>Mapping!$P6</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="16" t="str">
+        <f>Mapping!Q$11</f>
+        <v>Mange (10 eller mer)</v>
+      </c>
+      <c r="B19" s="37" t="str">
+        <f>Mapping!M$6</f>
+        <v>4 - Store</v>
+      </c>
+      <c r="C19" s="5">
+        <f>Mapping!$Q6</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="16" t="str">
+        <f>Mapping!N$11</f>
+        <v>Ett (1)</v>
+      </c>
+      <c r="B20" s="37" t="str">
+        <f>Mapping!M$5</f>
+        <v>5 - Svaert store</v>
+      </c>
+      <c r="C20" s="5">
+        <f>Mapping!$N5</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="16" t="str">
+        <f>Mapping!O$11</f>
+        <v>Noen (2-5)</v>
+      </c>
+      <c r="B21" s="37" t="str">
+        <f>Mapping!M$5</f>
+        <v>5 - Svaert store</v>
+      </c>
+      <c r="C21" s="5">
+        <f>Mapping!$O5</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="16" t="str">
+        <f>Mapping!P$11</f>
+        <v>Flere (6-10)</v>
+      </c>
+      <c r="B22" s="37" t="str">
+        <f>Mapping!M$5</f>
+        <v>5 - Svaert store</v>
+      </c>
+      <c r="C22" s="5">
+        <f>Mapping!$P5</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="16" t="str">
+        <f>Mapping!Q$11</f>
+        <v>Mange (10 eller mer)</v>
+      </c>
+      <c r="B23" s="37" t="str">
+        <f>Mapping!M$5</f>
+        <v>5 - Svaert store</v>
+      </c>
+      <c r="C23" s="5">
+        <f>Mapping!$Q5</f>
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
oppdatere configfil for skred mot faregrad plot
</commit_message>
<xml_diff>
--- a/varsomdata/input/aval_dl_configuration.xlsx
+++ b/varsomdata/input/aval_dl_configuration.xlsx
@@ -179,13 +179,13 @@
     <t>Observert faretegn</t>
   </si>
   <si>
-    <t xml:space="preserve">Vekting av en skredobservasjon. Høyere tall </t>
+    <t>order</t>
   </si>
   <si>
-    <t>betyr mer alvorlig situasjon.</t>
+    <t xml:space="preserve">Skredindex. Vekting av en skredobservasjon. </t>
   </si>
   <si>
-    <t>order</t>
+    <t>Høyere tall betyr mer alvorlig situasjon.</t>
   </si>
 </sst>
 </file>
@@ -796,12 +796,6 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -814,6 +808,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
   </cellXfs>
   <cellStyles count="389">
     <cellStyle name="Benyttet hyperkobling" xfId="3" builtinId="9" hidden="1"/>
@@ -7629,7 +7629,7 @@
   <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" customHeight="1"/>
@@ -7673,7 +7673,7 @@
       </c>
       <c r="F2" s="6"/>
       <c r="I2" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1">
@@ -7690,7 +7690,7 @@
         <v>100</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="15" customHeight="1">
@@ -7905,26 +7905,26 @@
       <c r="E11" s="4">
         <v>200</v>
       </c>
-      <c r="L11" s="30" t="str">
+      <c r="L11" s="36" t="str">
         <f>D10</f>
         <v>Ingen</v>
       </c>
-      <c r="M11" s="31" t="s">
+      <c r="M11" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="N11" s="30" t="str">
+      <c r="N11" s="36" t="str">
         <f>D12</f>
         <v>Ett (1)</v>
       </c>
-      <c r="O11" s="30" t="str">
+      <c r="O11" s="36" t="str">
         <f>D13</f>
         <v>Noen (2-5)</v>
       </c>
-      <c r="P11" s="30" t="str">
+      <c r="P11" s="36" t="str">
         <f>D14</f>
         <v>Flere (6-10)</v>
       </c>
-      <c r="Q11" s="30" t="str">
+      <c r="Q11" s="36" t="str">
         <f>D15</f>
         <v>Mange (10 eller mer)</v>
       </c>
@@ -7943,12 +7943,12 @@
       <c r="E12" s="4">
         <v>300</v>
       </c>
-      <c r="L12" s="30"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="30"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="30"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="36"/>
       <c r="S12" s="26"/>
     </row>
     <row r="13" spans="1:19" ht="15" customHeight="1">
@@ -7964,12 +7964,12 @@
       <c r="E13" s="4">
         <v>400</v>
       </c>
-      <c r="L13" s="30"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="30"/>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="30"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="36"/>
+      <c r="Q13" s="36"/>
     </row>
     <row r="14" spans="1:19" ht="15" customHeight="1">
       <c r="B14" s="4" t="s">
@@ -7984,12 +7984,12 @@
       <c r="E14" s="4">
         <v>500</v>
       </c>
-      <c r="L14" s="30"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="30"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="30"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="36"/>
     </row>
     <row r="15" spans="1:19" ht="15" customHeight="1">
       <c r="B15" s="4" t="s">
@@ -8004,12 +8004,12 @@
       <c r="E15" s="3">
         <v>600</v>
       </c>
-      <c r="L15" s="30"/>
-      <c r="M15" s="31"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="30"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="37"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="36"/>
     </row>
     <row r="16" spans="1:19" ht="15" customHeight="1">
       <c r="A16" s="6" t="s">
@@ -8022,12 +8022,12 @@
         <v>0</v>
       </c>
       <c r="F16" s="6"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="31"/>
-      <c r="N16" s="30"/>
-      <c r="O16" s="30"/>
-      <c r="P16" s="30"/>
-      <c r="Q16" s="30"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="36"/>
+      <c r="Q16" s="36"/>
     </row>
     <row r="17" spans="1:17" ht="15" customHeight="1">
       <c r="B17" s="4" t="s">
@@ -8042,12 +8042,12 @@
       <c r="E17" s="4">
         <v>0</v>
       </c>
-      <c r="L17" s="30"/>
-      <c r="M17" s="31"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="30"/>
-      <c r="P17" s="30"/>
-      <c r="Q17" s="30"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="36"/>
+      <c r="P17" s="36"/>
+      <c r="Q17" s="36"/>
     </row>
     <row r="18" spans="1:17" ht="15" customHeight="1">
       <c r="B18" s="4" t="s">
@@ -8062,12 +8062,12 @@
       <c r="E18" s="4">
         <v>600</v>
       </c>
-      <c r="L18" s="30"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="30"/>
-      <c r="P18" s="30"/>
-      <c r="Q18" s="30"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="37"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="36"/>
     </row>
     <row r="19" spans="1:17" ht="15" customHeight="1">
       <c r="B19" s="4" t="s">
@@ -8082,12 +8082,12 @@
       <c r="E19" s="4">
         <v>1200</v>
       </c>
-      <c r="L19" s="30"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="30"/>
-      <c r="O19" s="30"/>
-      <c r="P19" s="30"/>
-      <c r="Q19" s="30"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="36"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="36"/>
+      <c r="Q19" s="36"/>
     </row>
     <row r="20" spans="1:17" ht="15" customHeight="1">
       <c r="B20" s="4" t="s">
@@ -8228,22 +8228,22 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="20" style="16" customWidth="1"/>
-    <col min="2" max="2" width="16.625" style="35" customWidth="1"/>
+    <col min="2" max="2" width="16.625" style="33" customWidth="1"/>
     <col min="3" max="3" width="11" style="5"/>
     <col min="4" max="16384" width="11" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="32" t="str">
+      <c r="A1" s="30" t="str">
         <f>Mapping!A9</f>
         <v>EstimatedNum</v>
       </c>
-      <c r="B1" s="33" t="str">
+      <c r="B1" s="31" t="str">
         <f>Mapping!A2</f>
         <v>DestructiveSize</v>
       </c>
-      <c r="C1" s="34" t="s">
-        <v>54</v>
+      <c r="C1" s="32" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -8251,7 +8251,7 @@
         <f>Mapping!L11</f>
         <v>Ingen</v>
       </c>
-      <c r="B2" s="35" t="str">
+      <c r="B2" s="33" t="str">
         <f>A2</f>
         <v>Ingen</v>
       </c>
@@ -8261,11 +8261,11 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="36" t="str">
+      <c r="A3" s="34" t="str">
         <f>Mapping!M11</f>
         <v>Observert faretegn</v>
       </c>
-      <c r="B3" s="37" t="str">
+      <c r="B3" s="35" t="str">
         <f>A3</f>
         <v>Observert faretegn</v>
       </c>
@@ -8279,7 +8279,7 @@
         <f>Mapping!N$11</f>
         <v>Ett (1)</v>
       </c>
-      <c r="B4" s="37" t="str">
+      <c r="B4" s="35" t="str">
         <f>Mapping!M$9</f>
         <v>1 - Harmloest</v>
       </c>
@@ -8293,7 +8293,7 @@
         <f>Mapping!O$11</f>
         <v>Noen (2-5)</v>
       </c>
-      <c r="B5" s="37" t="str">
+      <c r="B5" s="35" t="str">
         <f>Mapping!M$9</f>
         <v>1 - Harmloest</v>
       </c>
@@ -8307,7 +8307,7 @@
         <f>Mapping!P$11</f>
         <v>Flere (6-10)</v>
       </c>
-      <c r="B6" s="37" t="str">
+      <c r="B6" s="35" t="str">
         <f>Mapping!M$9</f>
         <v>1 - Harmloest</v>
       </c>
@@ -8321,7 +8321,7 @@
         <f>Mapping!Q$11</f>
         <v>Mange (10 eller mer)</v>
       </c>
-      <c r="B7" s="37" t="str">
+      <c r="B7" s="35" t="str">
         <f>Mapping!M$9</f>
         <v>1 - Harmloest</v>
       </c>
@@ -8335,7 +8335,7 @@
         <f>Mapping!N$11</f>
         <v>Ett (1)</v>
       </c>
-      <c r="B8" s="37" t="str">
+      <c r="B8" s="35" t="str">
         <f>Mapping!M$8</f>
         <v>2 - Smaa</v>
       </c>
@@ -8349,7 +8349,7 @@
         <f>Mapping!O$11</f>
         <v>Noen (2-5)</v>
       </c>
-      <c r="B9" s="37" t="str">
+      <c r="B9" s="35" t="str">
         <f>Mapping!M$8</f>
         <v>2 - Smaa</v>
       </c>
@@ -8363,7 +8363,7 @@
         <f>Mapping!P$11</f>
         <v>Flere (6-10)</v>
       </c>
-      <c r="B10" s="37" t="str">
+      <c r="B10" s="35" t="str">
         <f>Mapping!M$8</f>
         <v>2 - Smaa</v>
       </c>
@@ -8377,7 +8377,7 @@
         <f>Mapping!Q$11</f>
         <v>Mange (10 eller mer)</v>
       </c>
-      <c r="B11" s="37" t="str">
+      <c r="B11" s="35" t="str">
         <f>Mapping!M$8</f>
         <v>2 - Smaa</v>
       </c>
@@ -8391,7 +8391,7 @@
         <f>Mapping!N$11</f>
         <v>Ett (1)</v>
       </c>
-      <c r="B12" s="37" t="str">
+      <c r="B12" s="35" t="str">
         <f>Mapping!M$7</f>
         <v>3 - Middels</v>
       </c>
@@ -8405,7 +8405,7 @@
         <f>Mapping!O$11</f>
         <v>Noen (2-5)</v>
       </c>
-      <c r="B13" s="37" t="str">
+      <c r="B13" s="35" t="str">
         <f>Mapping!M$7</f>
         <v>3 - Middels</v>
       </c>
@@ -8419,7 +8419,7 @@
         <f>Mapping!P$11</f>
         <v>Flere (6-10)</v>
       </c>
-      <c r="B14" s="37" t="str">
+      <c r="B14" s="35" t="str">
         <f>Mapping!M$7</f>
         <v>3 - Middels</v>
       </c>
@@ -8433,7 +8433,7 @@
         <f>Mapping!Q$11</f>
         <v>Mange (10 eller mer)</v>
       </c>
-      <c r="B15" s="37" t="str">
+      <c r="B15" s="35" t="str">
         <f>Mapping!M$7</f>
         <v>3 - Middels</v>
       </c>
@@ -8447,7 +8447,7 @@
         <f>Mapping!N$11</f>
         <v>Ett (1)</v>
       </c>
-      <c r="B16" s="37" t="str">
+      <c r="B16" s="35" t="str">
         <f>Mapping!M$6</f>
         <v>4 - Store</v>
       </c>
@@ -8461,7 +8461,7 @@
         <f>Mapping!O$11</f>
         <v>Noen (2-5)</v>
       </c>
-      <c r="B17" s="37" t="str">
+      <c r="B17" s="35" t="str">
         <f>Mapping!M$6</f>
         <v>4 - Store</v>
       </c>
@@ -8475,7 +8475,7 @@
         <f>Mapping!P$11</f>
         <v>Flere (6-10)</v>
       </c>
-      <c r="B18" s="37" t="str">
+      <c r="B18" s="35" t="str">
         <f>Mapping!M$6</f>
         <v>4 - Store</v>
       </c>
@@ -8489,7 +8489,7 @@
         <f>Mapping!Q$11</f>
         <v>Mange (10 eller mer)</v>
       </c>
-      <c r="B19" s="37" t="str">
+      <c r="B19" s="35" t="str">
         <f>Mapping!M$6</f>
         <v>4 - Store</v>
       </c>
@@ -8503,7 +8503,7 @@
         <f>Mapping!N$11</f>
         <v>Ett (1)</v>
       </c>
-      <c r="B20" s="37" t="str">
+      <c r="B20" s="35" t="str">
         <f>Mapping!M$5</f>
         <v>5 - Svaert store</v>
       </c>
@@ -8517,7 +8517,7 @@
         <f>Mapping!O$11</f>
         <v>Noen (2-5)</v>
       </c>
-      <c r="B21" s="37" t="str">
+      <c r="B21" s="35" t="str">
         <f>Mapping!M$5</f>
         <v>5 - Svaert store</v>
       </c>
@@ -8531,7 +8531,7 @@
         <f>Mapping!P$11</f>
         <v>Flere (6-10)</v>
       </c>
-      <c r="B22" s="37" t="str">
+      <c r="B22" s="35" t="str">
         <f>Mapping!M$5</f>
         <v>5 - Svaert store</v>
       </c>
@@ -8545,7 +8545,7 @@
         <f>Mapping!Q$11</f>
         <v>Mange (10 eller mer)</v>
       </c>
-      <c r="B23" s="37" t="str">
+      <c r="B23" s="35" t="str">
         <f>Mapping!M$5</f>
         <v>5 - Svaert store</v>
       </c>

</xml_diff>

<commit_message>
runavalancheactivity.py ferdig for denne gang.
</commit_message>
<xml_diff>
--- a/varsomdata/input/aval_dl_configuration.xlsx
+++ b/varsomdata/input/aval_dl_configuration.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-25245" yWindow="180" windowWidth="25605" windowHeight="16065" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="5160" yWindow="3020" windowWidth="29420" windowHeight="19680" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="aval_dl_configuration" sheetId="1" r:id="rId1"/>
+    <sheet name="aval_dl_configuration.csv" sheetId="1" r:id="rId1"/>
     <sheet name="Mapping" sheetId="2" r:id="rId2"/>
     <sheet name="aval_dl_order_of_size_and_num" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -158,9 +158,6 @@
     <t>unused cells</t>
   </si>
   <si>
-    <t>gray</t>
-  </si>
-  <si>
     <t>Danger sign</t>
   </si>
   <si>
@@ -171,9 +168,6 @@
   </si>
   <si>
     <t>No activity</t>
-  </si>
-  <si>
-    <t>blue</t>
   </si>
   <si>
     <t>Observert faretegn</t>
@@ -187,12 +181,18 @@
   <si>
     <t>Høyere tall betyr mer alvorlig situasjon.</t>
   </si>
+  <si>
+    <t>#729FCF</t>
+  </si>
+  <si>
+    <t>#E6E6E6</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -330,7 +330,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="389">
+  <cellStyleXfs count="397">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -622,6 +622,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -808,210 +816,214 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="180"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="389">
-    <cellStyle name="Benyttet hyperkobling" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="15" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="17" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="19" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="21" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="23" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="25" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="27" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="29" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="31" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="33" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="35" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="37" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="39" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="41" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="45" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="47" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="49" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="51" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="53" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="55" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="57" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="59" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="61" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="63" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="65" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="67" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="69" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="71" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="73" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="75" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="77" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="79" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="81" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="83" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="85" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="87" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="89" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="91" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="93" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="95" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="97" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="99" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="101" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="103" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="105" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="107" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="109" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="111" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="113" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="115" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="117" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="119" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="121" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="123" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="125" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="127" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="129" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="131" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="133" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="135" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="137" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="139" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="141" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="143" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="145" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="147" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="149" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="151" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="153" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="155" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="157" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="159" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="161" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="163" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="165" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="167" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="169" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="171" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="173" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="175" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="177" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="179" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="181" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="183" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="185" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="187" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="189" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="191" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="193" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="195" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="197" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="199" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="201" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="203" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="205" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="207" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="209" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="211" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="213" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="215" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="217" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="219" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="221" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="223" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="225" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="227" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="229" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="231" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="233" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="235" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="237" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="239" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="241" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="243" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="245" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="247" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="249" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="251" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="253" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="255" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="257" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="259" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="261" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="263" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="265" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="267" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="269" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="271" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="273" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="275" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="277" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="279" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="281" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="283" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="285" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="287" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="289" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="292" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="294" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="296" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="298" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="300" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="302" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="304" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="306" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="308" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="310" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="312" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="314" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="316" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="318" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="320" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="322" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="324" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="326" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="328" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="330" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="332" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="334" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="336" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="338" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="340" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="342" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="344" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="346" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="348" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="350" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="352" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="354" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="356" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="358" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="360" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="362" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="364" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="366" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="368" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="370" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="372" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="374" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="376" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="378" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="380" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="382" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="384" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="386" builtinId="9" hidden="1"/>
-    <cellStyle name="Benyttet hyperkobling" xfId="388" builtinId="9" hidden="1"/>
+  <cellStyles count="397">
     <cellStyle name="Dårlig" xfId="1" builtinId="27"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="207" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="209" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="211" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="213" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="215" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="217" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="245" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="247" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="249" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="251" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="253" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="255" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="257" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="259" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="261" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="263" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="265" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="267" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="269" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="271" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="273" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="275" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="277" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="279" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="281" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="283" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="285" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="287" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="289" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="366" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="368" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="370" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="372" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="374" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="376" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="378" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="380" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="382" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="384" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="386" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="388" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="392" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="394" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="396" builtinId="9" hidden="1"/>
     <cellStyle name="God" xfId="290" builtinId="26"/>
     <cellStyle name="Hyperkobling" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperkobling" xfId="4" builtinId="8" hidden="1"/>
@@ -1206,6 +1218,10 @@
     <cellStyle name="Hyperkobling" xfId="383" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperkobling" xfId="385" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperkobling" xfId="387" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperkobling" xfId="389" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperkobling" xfId="391" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperkobling" xfId="393" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperkobling" xfId="395" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1542,24 +1558,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H181"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A100" workbookViewId="0">
       <selection activeCell="L132" sqref="L132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.5" style="13" customWidth="1"/>
-    <col min="2" max="2" width="25.375" style="13" customWidth="1"/>
-    <col min="3" max="3" width="22.125" style="13" customWidth="1"/>
-    <col min="4" max="5" width="10.625" style="1" customWidth="1"/>
-    <col min="6" max="7" width="10.625" style="13" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="13"/>
+    <col min="2" max="2" width="25.33203125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" style="13" customWidth="1"/>
+    <col min="4" max="5" width="10.6640625" style="1" customWidth="1"/>
+    <col min="6" max="7" width="10.6640625" style="13" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="12" customFormat="1">
+    <row r="1" spans="1:8" s="12" customFormat="1" ht="16">
       <c r="A1" s="12" t="s">
         <v>15</v>
       </c>
@@ -1582,7 +1598,7 @@
         <v>1</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="24" customFormat="1">
@@ -1616,10 +1632,10 @@
       </c>
       <c r="H2" s="23" t="str">
         <f>Mapping!D$28</f>
-        <v>blue</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="12" customFormat="1">
+        <v>#729FCF</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="12" customFormat="1" ht="16">
       <c r="A3" s="13" t="str">
         <f>Mapping!D$17</f>
         <v>1 Liten</v>
@@ -1684,7 +1700,7 @@
       </c>
       <c r="H4" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="17" customFormat="1">
@@ -1718,7 +1734,7 @@
       </c>
       <c r="H5" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="17" customFormat="1">
@@ -1752,7 +1768,7 @@
       </c>
       <c r="H6" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="17" customFormat="1">
@@ -1786,7 +1802,7 @@
       </c>
       <c r="H7" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="17" customFormat="1">
@@ -1819,7 +1835,7 @@
       </c>
       <c r="H8" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="17" customFormat="1">
@@ -1852,7 +1868,7 @@
       </c>
       <c r="H9" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -2018,7 +2034,7 @@
       </c>
       <c r="H14" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="17" customFormat="1">
@@ -2051,7 +2067,7 @@
       </c>
       <c r="H15" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -2217,7 +2233,7 @@
       </c>
       <c r="H20" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="17" customFormat="1">
@@ -2250,7 +2266,7 @@
       </c>
       <c r="H21" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -2417,7 +2433,7 @@
       </c>
       <c r="H26" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="17" customFormat="1">
@@ -2451,7 +2467,7 @@
       </c>
       <c r="H27" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -2618,7 +2634,7 @@
       </c>
       <c r="H32" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="17" customFormat="1">
@@ -2652,7 +2668,7 @@
       </c>
       <c r="H33" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -2822,7 +2838,7 @@
       </c>
       <c r="H38" s="23" t="str">
         <f>Mapping!D$28</f>
-        <v>blue</v>
+        <v>#729FCF</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -2890,7 +2906,7 @@
       </c>
       <c r="H40" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="41" spans="1:8" s="1" customFormat="1">
@@ -2924,7 +2940,7 @@
       </c>
       <c r="H41" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="1" customFormat="1">
@@ -2958,7 +2974,7 @@
       </c>
       <c r="H42" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="43" spans="1:8" s="1" customFormat="1">
@@ -2992,7 +3008,7 @@
       </c>
       <c r="H43" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="1" customFormat="1">
@@ -3025,7 +3041,7 @@
       </c>
       <c r="H44" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="1" customFormat="1">
@@ -3058,7 +3074,7 @@
       </c>
       <c r="H45" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -3224,7 +3240,7 @@
       </c>
       <c r="H50" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="51" spans="1:8" s="1" customFormat="1">
@@ -3257,7 +3273,7 @@
       </c>
       <c r="H51" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -3423,7 +3439,7 @@
       </c>
       <c r="H56" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="57" spans="1:8" s="1" customFormat="1">
@@ -3456,7 +3472,7 @@
       </c>
       <c r="H57" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -3623,7 +3639,7 @@
       </c>
       <c r="H62" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="63" spans="1:8" s="1" customFormat="1">
@@ -3657,7 +3673,7 @@
       </c>
       <c r="H63" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -3824,7 +3840,7 @@
       </c>
       <c r="H68" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="69" spans="1:8" s="1" customFormat="1">
@@ -3858,7 +3874,7 @@
       </c>
       <c r="H69" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -4028,7 +4044,7 @@
       </c>
       <c r="H74" s="23" t="str">
         <f>Mapping!D$28</f>
-        <v>blue</v>
+        <v>#729FCF</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -4096,7 +4112,7 @@
       </c>
       <c r="H76" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="77" spans="1:8" s="1" customFormat="1">
@@ -4130,7 +4146,7 @@
       </c>
       <c r="H77" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="78" spans="1:8" s="1" customFormat="1">
@@ -4164,7 +4180,7 @@
       </c>
       <c r="H78" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="79" spans="1:8" s="1" customFormat="1">
@@ -4198,7 +4214,7 @@
       </c>
       <c r="H79" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="80" spans="1:8" s="1" customFormat="1">
@@ -4231,7 +4247,7 @@
       </c>
       <c r="H80" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="81" spans="1:8" s="1" customFormat="1">
@@ -4264,7 +4280,7 @@
       </c>
       <c r="H81" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -4430,7 +4446,7 @@
       </c>
       <c r="H86" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="87" spans="1:8" s="1" customFormat="1">
@@ -4463,7 +4479,7 @@
       </c>
       <c r="H87" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -4629,7 +4645,7 @@
       </c>
       <c r="H92" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="93" spans="1:8" s="1" customFormat="1">
@@ -4662,7 +4678,7 @@
       </c>
       <c r="H93" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -4829,7 +4845,7 @@
       </c>
       <c r="H98" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="99" spans="1:8" s="1" customFormat="1">
@@ -4863,7 +4879,7 @@
       </c>
       <c r="H99" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -5030,7 +5046,7 @@
       </c>
       <c r="H104" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="105" spans="1:8" s="1" customFormat="1">
@@ -5064,7 +5080,7 @@
       </c>
       <c r="H105" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="106" spans="1:8">
@@ -5234,7 +5250,7 @@
       </c>
       <c r="H110" s="23" t="str">
         <f>Mapping!D$28</f>
-        <v>blue</v>
+        <v>#729FCF</v>
       </c>
     </row>
     <row r="111" spans="1:8">
@@ -5302,7 +5318,7 @@
       </c>
       <c r="H112" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="113" spans="1:8" s="1" customFormat="1">
@@ -5336,7 +5352,7 @@
       </c>
       <c r="H113" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="114" spans="1:8" s="1" customFormat="1">
@@ -5370,7 +5386,7 @@
       </c>
       <c r="H114" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="115" spans="1:8" s="1" customFormat="1">
@@ -5404,7 +5420,7 @@
       </c>
       <c r="H115" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="116" spans="1:8" s="1" customFormat="1">
@@ -5437,7 +5453,7 @@
       </c>
       <c r="H116" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="117" spans="1:8" s="1" customFormat="1">
@@ -5470,7 +5486,7 @@
       </c>
       <c r="H117" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="118" spans="1:8">
@@ -5636,7 +5652,7 @@
       </c>
       <c r="H122" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="123" spans="1:8" s="1" customFormat="1">
@@ -5669,7 +5685,7 @@
       </c>
       <c r="H123" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="124" spans="1:8">
@@ -5835,7 +5851,7 @@
       </c>
       <c r="H128" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="129" spans="1:8" s="1" customFormat="1">
@@ -5868,7 +5884,7 @@
       </c>
       <c r="H129" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="130" spans="1:8">
@@ -6035,7 +6051,7 @@
       </c>
       <c r="H134" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="135" spans="1:8" s="1" customFormat="1">
@@ -6069,7 +6085,7 @@
       </c>
       <c r="H135" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="136" spans="1:8">
@@ -6236,7 +6252,7 @@
       </c>
       <c r="H140" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="141" spans="1:8" s="1" customFormat="1">
@@ -6270,7 +6286,7 @@
       </c>
       <c r="H141" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="142" spans="1:8">
@@ -6440,7 +6456,7 @@
       </c>
       <c r="H146" s="23" t="str">
         <f>Mapping!D$28</f>
-        <v>blue</v>
+        <v>#729FCF</v>
       </c>
     </row>
     <row r="147" spans="1:8">
@@ -6508,7 +6524,7 @@
       </c>
       <c r="H148" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="149" spans="1:8" s="1" customFormat="1">
@@ -6542,7 +6558,7 @@
       </c>
       <c r="H149" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="150" spans="1:8" s="1" customFormat="1">
@@ -6576,7 +6592,7 @@
       </c>
       <c r="H150" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="151" spans="1:8" s="1" customFormat="1">
@@ -6610,7 +6626,7 @@
       </c>
       <c r="H151" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="152" spans="1:8" s="1" customFormat="1">
@@ -6643,7 +6659,7 @@
       </c>
       <c r="H152" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="153" spans="1:8" s="1" customFormat="1">
@@ -6676,7 +6692,7 @@
       </c>
       <c r="H153" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="154" spans="1:8">
@@ -6842,7 +6858,7 @@
       </c>
       <c r="H158" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="159" spans="1:8" s="1" customFormat="1">
@@ -6875,7 +6891,7 @@
       </c>
       <c r="H159" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="160" spans="1:8">
@@ -7041,7 +7057,7 @@
       </c>
       <c r="H164" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="165" spans="1:8" s="1" customFormat="1">
@@ -7074,7 +7090,7 @@
       </c>
       <c r="H165" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="166" spans="1:8">
@@ -7241,7 +7257,7 @@
       </c>
       <c r="H170" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="171" spans="1:8" s="1" customFormat="1">
@@ -7275,7 +7291,7 @@
       </c>
       <c r="H171" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="172" spans="1:8">
@@ -7442,7 +7458,7 @@
       </c>
       <c r="H176" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="177" spans="1:8" s="1" customFormat="1">
@@ -7476,7 +7492,7 @@
       </c>
       <c r="H177" s="1" t="str">
         <f>Mapping!D$27</f>
-        <v>gray</v>
+        <v>#E6E6E6</v>
       </c>
     </row>
     <row r="178" spans="1:8">
@@ -7627,27 +7643,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="4" customWidth="1"/>
     <col min="3" max="3" width="6.5" style="5" customWidth="1"/>
     <col min="4" max="4" width="17.5" style="16" customWidth="1"/>
-    <col min="5" max="5" width="10.875" style="4"/>
-    <col min="6" max="6" width="24.875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="10.875" style="3"/>
-    <col min="8" max="19" width="3.875" style="3" customWidth="1"/>
-    <col min="20" max="16384" width="10.875" style="3"/>
+    <col min="5" max="5" width="10.83203125" style="4"/>
+    <col min="6" max="6" width="24.83203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="3"/>
+    <col min="8" max="19" width="3.83203125" style="3" customWidth="1"/>
+    <col min="20" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:22" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -7661,7 +7677,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="9"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1">
+    <row r="2" spans="1:22" ht="15" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>29</v>
       </c>
@@ -7675,10 +7691,10 @@
       </c>
       <c r="F2" s="6"/>
       <c r="I2" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="15" customHeight="1">
       <c r="B3" s="4">
         <v>0</v>
       </c>
@@ -7692,10 +7708,10 @@
         <v>100</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="15" customHeight="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="15" customHeight="1">
       <c r="B4" s="4">
         <v>1</v>
       </c>
@@ -7708,8 +7724,18 @@
       <c r="E4" s="4">
         <v>200</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" ht="15" customHeight="1">
+      <c r="T4" s="3">
+        <v>564</v>
+      </c>
+      <c r="U4" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="V4" s="3">
+        <f>U4*T4</f>
+        <v>90.24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="15" customHeight="1">
       <c r="B5" s="4">
         <v>2</v>
       </c>
@@ -7738,8 +7764,18 @@
       <c r="Q5" s="5">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" ht="15" customHeight="1">
+      <c r="T5" s="3">
+        <v>2438</v>
+      </c>
+      <c r="U5" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="V5" s="3">
+        <f t="shared" ref="V5:V7" si="0">U5*T5</f>
+        <v>707.02</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="15" customHeight="1">
       <c r="B6" s="4">
         <v>3</v>
       </c>
@@ -7769,8 +7805,18 @@
       <c r="Q6" s="5">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" ht="15" customHeight="1">
+      <c r="T6" s="3">
+        <v>1021</v>
+      </c>
+      <c r="U6" s="3">
+        <v>0.44</v>
+      </c>
+      <c r="V6" s="3">
+        <f t="shared" si="0"/>
+        <v>449.24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="15" customHeight="1">
       <c r="B7" s="4">
         <v>4</v>
       </c>
@@ -7800,8 +7846,18 @@
       <c r="Q7" s="5">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1">
+      <c r="T7" s="3">
+        <v>79</v>
+      </c>
+      <c r="U7" s="3">
+        <v>0.48</v>
+      </c>
+      <c r="V7" s="3">
+        <f t="shared" si="0"/>
+        <v>37.92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="15" customHeight="1">
       <c r="B8" s="4">
         <v>5</v>
       </c>
@@ -7831,8 +7887,16 @@
       <c r="Q8" s="5">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" ht="15" customHeight="1">
+      <c r="T8" s="3">
+        <f>SUM(T4:T7)</f>
+        <v>4102</v>
+      </c>
+      <c r="V8" s="3">
+        <f>SUM(V4:V7)</f>
+        <v>1284.42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="15" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>28</v>
       </c>
@@ -7861,7 +7925,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="15" customHeight="1">
+    <row r="10" spans="1:22" ht="15" customHeight="1">
       <c r="B10" s="4" t="s">
         <v>39</v>
       </c>
@@ -7874,7 +7938,7 @@
       <c r="E10" s="4">
         <v>100</v>
       </c>
-      <c r="K10" s="37" t="s">
+      <c r="K10" s="35" t="s">
         <v>38</v>
       </c>
       <c r="L10" s="5">
@@ -7896,45 +7960,45 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1">
+    <row r="11" spans="1:22" ht="15" customHeight="1">
       <c r="B11" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11" s="4">
         <v>200</v>
       </c>
-      <c r="L11" s="35" t="str">
+      <c r="L11" s="36" t="str">
         <f>D10</f>
         <v>Ingen</v>
       </c>
-      <c r="M11" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="N11" s="35" t="str">
+      <c r="M11" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="N11" s="36" t="str">
         <f>D12</f>
         <v>Ett (1)</v>
       </c>
-      <c r="O11" s="35" t="str">
+      <c r="O11" s="36" t="str">
         <f>D13</f>
         <v>Noen (2-5)</v>
       </c>
-      <c r="P11" s="35" t="str">
+      <c r="P11" s="36" t="str">
         <f>D14</f>
         <v>Flere (6-10)</v>
       </c>
-      <c r="Q11" s="35" t="str">
+      <c r="Q11" s="36" t="str">
         <f>D15</f>
         <v>Mange (10 eller mer)</v>
       </c>
       <c r="S11" s="26"/>
     </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1">
+    <row r="12" spans="1:22" ht="15" customHeight="1">
       <c r="B12" s="4" t="s">
         <v>24</v>
       </c>
@@ -7947,15 +8011,15 @@
       <c r="E12" s="4">
         <v>300</v>
       </c>
-      <c r="L12" s="35"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="35"/>
-      <c r="O12" s="35"/>
-      <c r="P12" s="35"/>
-      <c r="Q12" s="35"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="36"/>
       <c r="S12" s="25"/>
     </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1">
+    <row r="13" spans="1:22" ht="15" customHeight="1">
       <c r="B13" s="4" t="s">
         <v>25</v>
       </c>
@@ -7968,14 +8032,14 @@
       <c r="E13" s="4">
         <v>400</v>
       </c>
-      <c r="L13" s="35"/>
-      <c r="M13" s="36"/>
-      <c r="N13" s="35"/>
-      <c r="O13" s="35"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="35"/>
-    </row>
-    <row r="14" spans="1:19" ht="15" customHeight="1">
+      <c r="L13" s="36"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="36"/>
+      <c r="Q13" s="36"/>
+    </row>
+    <row r="14" spans="1:22" ht="15" customHeight="1">
       <c r="B14" s="4" t="s">
         <v>26</v>
       </c>
@@ -7988,14 +8052,14 @@
       <c r="E14" s="4">
         <v>500</v>
       </c>
-      <c r="L14" s="35"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
-    </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1">
+      <c r="L14" s="36"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="36"/>
+    </row>
+    <row r="15" spans="1:22" ht="15" customHeight="1">
       <c r="B15" s="4" t="s">
         <v>27</v>
       </c>
@@ -8008,14 +8072,14 @@
       <c r="E15" s="3">
         <v>600</v>
       </c>
-      <c r="L15" s="35"/>
-      <c r="M15" s="36"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="35"/>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="35"/>
-    </row>
-    <row r="16" spans="1:19" ht="15" customHeight="1">
+      <c r="L15" s="36"/>
+      <c r="M15" s="37"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="36"/>
+    </row>
+    <row r="16" spans="1:22" ht="15" customHeight="1">
       <c r="A16" s="6" t="s">
         <v>30</v>
       </c>
@@ -8026,12 +8090,12 @@
         <v>0</v>
       </c>
       <c r="F16" s="6"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="36"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="35"/>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="35"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="36"/>
+      <c r="Q16" s="36"/>
     </row>
     <row r="17" spans="1:17" ht="15" customHeight="1">
       <c r="B17" s="4" t="s">
@@ -8046,12 +8110,12 @@
       <c r="E17" s="4">
         <v>0</v>
       </c>
-      <c r="L17" s="35"/>
-      <c r="M17" s="36"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="36"/>
+      <c r="P17" s="36"/>
+      <c r="Q17" s="36"/>
     </row>
     <row r="18" spans="1:17" ht="15" customHeight="1">
       <c r="B18" s="4" t="s">
@@ -8066,12 +8130,12 @@
       <c r="E18" s="4">
         <v>600</v>
       </c>
-      <c r="L18" s="35"/>
-      <c r="M18" s="36"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="37"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="36"/>
     </row>
     <row r="19" spans="1:17" ht="15" customHeight="1">
       <c r="B19" s="4" t="s">
@@ -8086,12 +8150,12 @@
       <c r="E19" s="4">
         <v>1200</v>
       </c>
-      <c r="L19" s="35"/>
-      <c r="M19" s="36"/>
-      <c r="N19" s="35"/>
-      <c r="O19" s="35"/>
-      <c r="P19" s="35"/>
-      <c r="Q19" s="35"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="36"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="36"/>
+      <c r="Q19" s="36"/>
     </row>
     <row r="20" spans="1:17" ht="15" customHeight="1">
       <c r="B20" s="4" t="s">
@@ -8186,20 +8250,20 @@
         <v>42</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
     </row>
     <row r="28" spans="1:17" ht="15" customHeight="1">
       <c r="B28" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C28" s="22" t="s">
         <v>42</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -8212,7 +8276,7 @@
     <mergeCell ref="N11:N19"/>
   </mergeCells>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -8222,19 +8286,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20" style="16" customWidth="1"/>
-    <col min="2" max="2" width="16.625" style="32" customWidth="1"/>
-    <col min="3" max="3" width="11" style="5"/>
-    <col min="4" max="16384" width="11" style="3"/>
+    <col min="2" max="2" width="16.6640625" style="32" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="5"/>
+    <col min="4" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -8247,7 +8311,7 @@
         <v>DestructiveSize</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -8560,6 +8624,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
runlevelanddangersign.py complete. Some changes to the get methods
</commit_message>
<xml_diff>
--- a/varsomdata/input/aval_dl_configuration.xlsx
+++ b/varsomdata/input/aval_dl_configuration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5160" yWindow="3020" windowWidth="29420" windowHeight="19680" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="aval_dl_configuration.csv" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="65">
   <si>
     <t>x</t>
   </si>
@@ -187,6 +187,36 @@
   <si>
     <t>#E6E6E6</t>
   </si>
+  <si>
+    <t>fg 1</t>
+  </si>
+  <si>
+    <t>fg 2</t>
+  </si>
+  <si>
+    <t>fg 3</t>
+  </si>
+  <si>
+    <t>fg 5</t>
+  </si>
+  <si>
+    <t>fg 4</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>#ff0000</t>
+  </si>
+  <si>
+    <t>#ff9900</t>
+  </si>
+  <si>
+    <t>#ffff00</t>
+  </si>
+  <si>
+    <t>#ccff66</t>
+  </si>
 </sst>
 </file>
 
@@ -330,7 +360,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="397">
+  <cellStyleXfs count="409">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -622,6 +652,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -825,7 +867,7 @@
       <alignment horizontal="center" vertical="top" textRotation="180"/>
     </xf>
   </cellXfs>
-  <cellStyles count="397">
+  <cellStyles count="409">
     <cellStyle name="Dårlig" xfId="1" builtinId="27"/>
     <cellStyle name="Fulgt hyperkobling" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Fulgt hyperkobling" xfId="5" builtinId="9" hidden="1"/>
@@ -1024,6 +1066,12 @@
     <cellStyle name="Fulgt hyperkobling" xfId="392" builtinId="9" hidden="1"/>
     <cellStyle name="Fulgt hyperkobling" xfId="394" builtinId="9" hidden="1"/>
     <cellStyle name="Fulgt hyperkobling" xfId="396" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="398" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="400" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="402" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="404" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="406" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="408" builtinId="9" hidden="1"/>
     <cellStyle name="God" xfId="290" builtinId="26"/>
     <cellStyle name="Hyperkobling" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperkobling" xfId="4" builtinId="8" hidden="1"/>
@@ -1222,6 +1270,12 @@
     <cellStyle name="Hyperkobling" xfId="391" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperkobling" xfId="393" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperkobling" xfId="395" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperkobling" xfId="397" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperkobling" xfId="399" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperkobling" xfId="401" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperkobling" xfId="403" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperkobling" xfId="405" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperkobling" xfId="407" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1561,8 +1615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H181"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="L132" sqref="L132"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1665,8 +1719,8 @@
         <v>100</v>
       </c>
       <c r="H3" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$29</f>
+        <v>#ccff66</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="17" customFormat="1">
@@ -1900,8 +1954,8 @@
         <v>200</v>
       </c>
       <c r="H10" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$29</f>
+        <v>#ccff66</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1933,8 +1987,8 @@
         <v>200</v>
       </c>
       <c r="H11" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$29</f>
+        <v>#ccff66</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2099,8 +2153,8 @@
         <v>300</v>
       </c>
       <c r="H16" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$29</f>
+        <v>#ccff66</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2132,8 +2186,8 @@
         <v>300</v>
       </c>
       <c r="H17" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$29</f>
+        <v>#ccff66</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -2871,8 +2925,8 @@
         <v>100</v>
       </c>
       <c r="H39" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$30</f>
+        <v>#ffff00</v>
       </c>
     </row>
     <row r="40" spans="1:8" s="1" customFormat="1">
@@ -3106,8 +3160,8 @@
         <v>200</v>
       </c>
       <c r="H46" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$30</f>
+        <v>#ffff00</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -3139,8 +3193,8 @@
         <v>200</v>
       </c>
       <c r="H47" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$30</f>
+        <v>#ffff00</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -3173,8 +3227,8 @@
         <v>200</v>
       </c>
       <c r="H48" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$30</f>
+        <v>#ffff00</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -3206,8 +3260,8 @@
         <v>200</v>
       </c>
       <c r="H49" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$30</f>
+        <v>#ffff00</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="1" customFormat="1">
@@ -3305,8 +3359,8 @@
         <v>300</v>
       </c>
       <c r="H52" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$30</f>
+        <v>#ffff00</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -3338,8 +3392,8 @@
         <v>300</v>
       </c>
       <c r="H53" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$30</f>
+        <v>#ffff00</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -3372,8 +3426,8 @@
         <v>300</v>
       </c>
       <c r="H54" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$30</f>
+        <v>#ffff00</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -3504,8 +3558,8 @@
         <v>400</v>
       </c>
       <c r="H58" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$30</f>
+        <v>#ffff00</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -3537,8 +3591,8 @@
         <v>400</v>
       </c>
       <c r="H59" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$30</f>
+        <v>#ffff00</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -4077,8 +4131,8 @@
         <v>100</v>
       </c>
       <c r="H75" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$31</f>
+        <v>#ff9900</v>
       </c>
     </row>
     <row r="76" spans="1:8" s="1" customFormat="1">
@@ -4312,8 +4366,8 @@
         <v>200</v>
       </c>
       <c r="H82" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$31</f>
+        <v>#ff9900</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -4345,8 +4399,8 @@
         <v>200</v>
       </c>
       <c r="H83" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$31</f>
+        <v>#ff9900</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -4379,8 +4433,8 @@
         <v>200</v>
       </c>
       <c r="H84" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$31</f>
+        <v>#ff9900</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -4412,8 +4466,8 @@
         <v>200</v>
       </c>
       <c r="H85" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$31</f>
+        <v>#ff9900</v>
       </c>
     </row>
     <row r="86" spans="1:8" s="1" customFormat="1">
@@ -4511,8 +4565,8 @@
         <v>300</v>
       </c>
       <c r="H88" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$31</f>
+        <v>#ff9900</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -4544,8 +4598,8 @@
         <v>300</v>
       </c>
       <c r="H89" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$31</f>
+        <v>#ff9900</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -4578,8 +4632,8 @@
         <v>300</v>
       </c>
       <c r="H90" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$31</f>
+        <v>#ff9900</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -4710,8 +4764,8 @@
         <v>400</v>
       </c>
       <c r="H94" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$31</f>
+        <v>#ff9900</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -4743,8 +4797,8 @@
         <v>400</v>
       </c>
       <c r="H95" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$31</f>
+        <v>#ff9900</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -4911,8 +4965,8 @@
         <v>500</v>
       </c>
       <c r="H100" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$31</f>
+        <v>#ff9900</v>
       </c>
     </row>
     <row r="101" spans="1:8">
@@ -5283,8 +5337,8 @@
         <v>100</v>
       </c>
       <c r="H111" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$32</f>
+        <v>#ff0000</v>
       </c>
     </row>
     <row r="112" spans="1:8" s="1" customFormat="1">
@@ -5518,8 +5572,8 @@
         <v>200</v>
       </c>
       <c r="H118" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$32</f>
+        <v>#ff0000</v>
       </c>
     </row>
     <row r="119" spans="1:8">
@@ -5551,8 +5605,8 @@
         <v>200</v>
       </c>
       <c r="H119" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$32</f>
+        <v>#ff0000</v>
       </c>
     </row>
     <row r="120" spans="1:8">
@@ -5585,8 +5639,8 @@
         <v>200</v>
       </c>
       <c r="H120" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$32</f>
+        <v>#ff0000</v>
       </c>
     </row>
     <row r="121" spans="1:8">
@@ -5618,8 +5672,8 @@
         <v>200</v>
       </c>
       <c r="H121" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$32</f>
+        <v>#ff0000</v>
       </c>
     </row>
     <row r="122" spans="1:8" s="1" customFormat="1">
@@ -5717,8 +5771,8 @@
         <v>300</v>
       </c>
       <c r="H124" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$32</f>
+        <v>#ff0000</v>
       </c>
     </row>
     <row r="125" spans="1:8">
@@ -5750,8 +5804,8 @@
         <v>300</v>
       </c>
       <c r="H125" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$32</f>
+        <v>#ff0000</v>
       </c>
     </row>
     <row r="126" spans="1:8">
@@ -5784,8 +5838,8 @@
         <v>300</v>
       </c>
       <c r="H126" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$32</f>
+        <v>#ff0000</v>
       </c>
     </row>
     <row r="127" spans="1:8">
@@ -5817,8 +5871,8 @@
         <v>300</v>
       </c>
       <c r="H127" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$32</f>
+        <v>#ff0000</v>
       </c>
     </row>
     <row r="128" spans="1:8" s="1" customFormat="1">
@@ -5916,8 +5970,8 @@
         <v>400</v>
       </c>
       <c r="H130" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$32</f>
+        <v>#ff0000</v>
       </c>
     </row>
     <row r="131" spans="1:8">
@@ -5949,8 +6003,8 @@
         <v>400</v>
       </c>
       <c r="H131" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$32</f>
+        <v>#ff0000</v>
       </c>
     </row>
     <row r="132" spans="1:8">
@@ -5983,8 +6037,8 @@
         <v>400</v>
       </c>
       <c r="H132" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$32</f>
+        <v>#ff0000</v>
       </c>
     </row>
     <row r="133" spans="1:8">
@@ -6016,8 +6070,8 @@
         <v>400</v>
       </c>
       <c r="H133" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$32</f>
+        <v>#ff0000</v>
       </c>
     </row>
     <row r="134" spans="1:8" s="1" customFormat="1">
@@ -6117,8 +6171,8 @@
         <v>500</v>
       </c>
       <c r="H136" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$32</f>
+        <v>#ff0000</v>
       </c>
     </row>
     <row r="137" spans="1:8">
@@ -6150,8 +6204,8 @@
         <v>500</v>
       </c>
       <c r="H137" s="18" t="str">
-        <f>Mapping!D$26</f>
-        <v>white</v>
+        <f>Mapping!D$32</f>
+        <v>#ff0000</v>
       </c>
     </row>
     <row r="138" spans="1:8">
@@ -7644,10 +7698,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V28"/>
+  <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -8264,6 +8318,61 @@
       </c>
       <c r="D28" s="16" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="15" customHeight="1">
+      <c r="B29" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="15" customHeight="1">
+      <c r="B30" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="15" customHeight="1">
+      <c r="B31" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="15" customHeight="1">
+      <c r="B32" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="15" customHeight="1">
+      <c r="B33" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new danger and problem with avalindex
</commit_message>
<xml_diff>
--- a/varsomdata/input/aval_dl_configuration.xlsx
+++ b/varsomdata/input/aval_dl_configuration.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="7820" yWindow="3120" windowWidth="25520" windowHeight="15600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="aval_dl_configuration.csv" sheetId="1" r:id="rId1"/>
@@ -309,7 +309,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -350,6 +350,36 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFA98"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF683FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -771,7 +801,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -865,6 +895,21 @@
     </xf>
     <xf numFmtId="49" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="409">
@@ -1615,7 +1660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
@@ -7700,8 +7745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -7806,16 +7851,16 @@
         <f>D8</f>
         <v>5 - Svaert store</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="41">
         <v>14</v>
       </c>
-      <c r="O5" s="5">
+      <c r="O5" s="41">
         <v>18</v>
       </c>
-      <c r="P5" s="5">
+      <c r="P5" s="41">
         <v>21</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="Q5" s="41">
         <v>22</v>
       </c>
       <c r="T5" s="3">
@@ -7847,17 +7892,17 @@
         <f>D7</f>
         <v>4 - Store</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="40">
         <v>10</v>
       </c>
-      <c r="O6" s="5">
+      <c r="O6" s="41">
         <v>15</v>
       </c>
-      <c r="P6" s="5">
+      <c r="P6" s="41">
         <v>19</v>
       </c>
-      <c r="Q6" s="5">
-        <v>19</v>
+      <c r="Q6" s="41">
+        <v>20</v>
       </c>
       <c r="T6" s="3">
         <v>1021</v>
@@ -7888,16 +7933,16 @@
         <f>D6</f>
         <v>3 - Middels</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="39">
         <v>6</v>
       </c>
-      <c r="O7" s="5">
+      <c r="O7" s="40">
         <v>11</v>
       </c>
-      <c r="P7" s="5">
+      <c r="P7" s="41">
         <v>16</v>
       </c>
-      <c r="Q7" s="5">
+      <c r="Q7" s="41">
         <v>17</v>
       </c>
       <c r="T7" s="3">
@@ -7929,16 +7974,16 @@
         <f>D5</f>
         <v>2 - Smaa</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="38">
         <v>4</v>
       </c>
-      <c r="O8" s="5">
+      <c r="O8" s="40">
         <v>9</v>
       </c>
-      <c r="P8" s="5">
+      <c r="P8" s="40">
         <v>12</v>
       </c>
-      <c r="Q8" s="5">
+      <c r="Q8" s="41">
         <v>13</v>
       </c>
       <c r="T8" s="3">
@@ -7966,16 +8011,16 @@
         <f>D4</f>
         <v>1 - Harmloest</v>
       </c>
-      <c r="N9" s="5">
+      <c r="N9" s="38">
         <v>3</v>
       </c>
-      <c r="O9" s="5">
+      <c r="O9" s="38">
         <v>5</v>
       </c>
-      <c r="P9" s="5">
+      <c r="P9" s="39">
         <v>7</v>
       </c>
-      <c r="Q9" s="5">
+      <c r="Q9" s="39">
         <v>8</v>
       </c>
     </row>
@@ -7995,10 +8040,10 @@
       <c r="K10" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L10" s="42">
         <v>1</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10" s="38">
         <v>2</v>
       </c>
       <c r="N10" s="28">
@@ -8672,7 +8717,7 @@
       </c>
       <c r="C19" s="5">
         <f>Mapping!$Q6</f>
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:3">

</xml_diff>

<commit_message>
Make avalanche activity plot for 2015-16
</commit_message>
<xml_diff>
--- a/varsomdata/input/aval_dl_configuration.xlsx
+++ b/varsomdata/input/aval_dl_configuration.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raek\github\varsomdata\varsomdata\input\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7820" yWindow="3120" windowWidth="25520" windowHeight="15600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="7815" yWindow="3120" windowWidth="25515" windowHeight="15600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="aval_dl_configuration.csv" sheetId="1" r:id="rId1"/>
     <sheet name="Mapping" sheetId="2" r:id="rId2"/>
     <sheet name="aval_dl_order_of_size_and_num" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -222,7 +227,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -913,210 +918,210 @@
     </xf>
   </cellXfs>
   <cellStyles count="409">
+    <cellStyle name="Benyttet hyperkobling" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="207" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="209" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="211" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="213" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="215" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="217" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="245" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="247" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="249" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="251" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="253" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="255" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="257" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="259" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="261" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="263" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="265" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="267" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="269" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="271" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="273" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="275" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="277" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="279" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="281" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="283" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="285" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="287" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="289" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="366" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="368" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="370" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="372" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="374" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="376" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="378" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="380" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="382" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="384" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="386" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="388" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="392" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="394" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="396" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="398" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="400" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="402" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="404" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="406" builtinId="9" hidden="1"/>
+    <cellStyle name="Benyttet hyperkobling" xfId="408" builtinId="9" hidden="1"/>
     <cellStyle name="Dårlig" xfId="1" builtinId="27"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="15" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="17" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="19" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="21" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="23" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="25" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="27" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="29" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="31" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="33" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="35" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="37" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="39" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="41" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="45" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="47" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="49" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="51" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="53" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="55" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="57" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="59" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="61" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="63" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="65" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="67" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="69" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="71" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="73" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="75" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="77" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="79" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="81" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="83" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="85" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="87" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="89" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="91" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="93" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="95" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="97" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="99" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="101" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="103" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="105" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="107" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="109" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="111" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="113" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="115" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="117" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="119" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="121" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="123" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="125" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="127" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="129" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="131" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="133" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="135" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="137" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="139" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="141" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="143" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="145" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="147" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="149" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="151" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="153" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="155" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="157" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="159" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="161" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="163" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="165" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="167" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="169" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="171" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="173" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="175" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="177" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="179" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="181" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="183" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="185" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="187" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="189" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="191" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="193" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="195" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="197" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="199" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="201" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="203" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="205" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="207" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="209" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="211" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="213" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="215" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="217" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="219" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="221" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="223" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="225" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="227" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="229" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="231" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="233" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="235" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="237" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="239" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="241" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="243" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="245" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="247" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="249" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="251" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="253" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="255" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="257" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="259" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="261" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="263" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="265" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="267" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="269" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="271" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="273" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="275" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="277" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="279" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="281" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="283" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="285" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="287" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="289" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="292" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="294" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="296" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="298" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="300" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="302" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="304" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="306" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="308" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="310" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="312" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="314" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="316" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="318" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="320" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="322" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="324" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="326" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="328" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="330" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="332" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="334" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="336" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="338" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="340" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="342" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="344" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="346" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="348" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="350" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="352" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="354" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="356" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="358" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="360" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="362" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="364" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="366" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="368" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="370" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="372" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="374" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="376" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="378" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="380" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="382" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="384" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="386" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="388" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="390" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="392" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="394" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="396" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="398" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="400" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="402" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="404" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="406" builtinId="9" hidden="1"/>
-    <cellStyle name="Fulgt hyperkobling" xfId="408" builtinId="9" hidden="1"/>
     <cellStyle name="God" xfId="290" builtinId="26"/>
     <cellStyle name="Hyperkobling" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperkobling" xfId="4" builtinId="8" hidden="1"/>
@@ -1664,17 +1669,17 @@
       <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="16.5" style="13" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" style="13" customWidth="1"/>
-    <col min="4" max="5" width="10.6640625" style="1" customWidth="1"/>
-    <col min="6" max="7" width="10.6640625" style="13" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="13"/>
+    <col min="2" max="2" width="25.375" style="13" customWidth="1"/>
+    <col min="3" max="3" width="22.125" style="13" customWidth="1"/>
+    <col min="4" max="5" width="10.625" style="1" customWidth="1"/>
+    <col min="6" max="7" width="10.625" style="13" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="12" customFormat="1" ht="16">
+    <row r="1" spans="1:8" s="12" customFormat="1">
       <c r="A1" s="12" t="s">
         <v>15</v>
       </c>
@@ -1734,7 +1739,7 @@
         <v>#729FCF</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" ht="16">
+    <row r="3" spans="1:8" s="12" customFormat="1">
       <c r="A3" s="13" t="str">
         <f>Mapping!D$17</f>
         <v>1 Liten</v>
@@ -7745,21 +7750,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="14" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.375" style="4" customWidth="1"/>
     <col min="3" max="3" width="6.5" style="5" customWidth="1"/>
     <col min="4" max="4" width="17.5" style="16" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="4"/>
-    <col min="6" max="6" width="24.83203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="3"/>
-    <col min="8" max="19" width="3.83203125" style="3" customWidth="1"/>
-    <col min="20" max="16384" width="10.83203125" style="3"/>
+    <col min="5" max="5" width="10.875" style="4"/>
+    <col min="6" max="6" width="24.875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.875" style="3"/>
+    <col min="8" max="19" width="3.875" style="3" customWidth="1"/>
+    <col min="20" max="16384" width="10.875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="2" customFormat="1" ht="15" customHeight="1">
@@ -8447,12 +8452,12 @@
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="20" style="16" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" style="32" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="5"/>
-    <col min="4" max="16384" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="16.625" style="32" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="5"/>
+    <col min="4" max="16384" width="10.875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>